<commit_message>
added Mozilla Public License info
</commit_message>
<xml_diff>
--- a/xlsx2owl-Example.xlsx
+++ b/xlsx2owl-Example.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CE51C8A-9BFE-4CEB-81C5-3F023D31830B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF5DB2C9-F2D6-46D9-9700-44B63472FF55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1815" yWindow="1815" windowWidth="21600" windowHeight="11385" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Classes" sheetId="1" r:id="rId1"/>
@@ -481,7 +481,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="77">
   <si>
     <t>Domain</t>
   </si>
@@ -706,13 +706,19 @@
   </si>
   <si>
     <t>base</t>
+  </si>
+  <si>
+    <t>License</t>
+  </si>
+  <si>
+    <t>This Spreadsheet is subject to the terms of the Mozilla Public License, v. 2.0. If a copy of the MPL was not distributed with this file, You can obtain one at https://mozilla.org/MPL/2.0/.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -798,6 +804,13 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="10">
     <fill>
@@ -878,7 +891,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -889,16 +902,16 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -918,13 +931,12 @@
     <xf numFmtId="49" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -960,6 +972,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1673,7 +1691,7 @@
   </sheetPr>
   <dimension ref="A1:J83"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="F7" sqref="F7"/>
       <selection pane="topRight"/>
@@ -1886,14 +1904,14 @@
     <col min="3" max="3" width="16.5" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="23" customFormat="1" ht="18.75">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:3" s="22" customFormat="1" ht="18.75">
+      <c r="A1" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="23" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1911,72 +1929,79 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A2:D10"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="25.875" style="25" customWidth="1"/>
-    <col min="2" max="2" width="10" style="25" customWidth="1"/>
+    <col min="1" max="1" width="92.25" style="24" customWidth="1"/>
+    <col min="2" max="2" width="10" style="24" customWidth="1"/>
     <col min="3" max="3" width="106.625" customWidth="1"/>
     <col min="4" max="4" width="11.625" style="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" ht="23.25">
-      <c r="A2" s="26"/>
-      <c r="C2" s="27"/>
+    <row r="1" spans="1:4">
+      <c r="A1" s="35" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="31.5">
+      <c r="A2" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="26"/>
     </row>
     <row r="3" spans="1:4" ht="23.25">
-      <c r="A3" s="26"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="29"/>
+      <c r="A3" s="25"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="28"/>
     </row>
     <row r="4" spans="1:4" ht="23.25">
-      <c r="A4" s="28"/>
-      <c r="B4" s="28"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="29"/>
+      <c r="A4" s="27"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="28"/>
     </row>
     <row r="5" spans="1:4" ht="23.25">
-      <c r="A5" s="26"/>
-      <c r="B5" s="28"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="29"/>
-    </row>
-    <row r="6" spans="1:4" s="31" customFormat="1">
-      <c r="A6" s="26"/>
-      <c r="B6" s="26"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="33"/>
+      <c r="A5" s="25"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="28"/>
+    </row>
+    <row r="6" spans="1:4" s="30" customFormat="1">
+      <c r="A6" s="25"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="32"/>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="28"/>
-      <c r="B7" s="28"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="29"/>
+      <c r="A7" s="27"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="28"/>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="28"/>
-      <c r="B8" s="28"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="29"/>
+      <c r="A8" s="27"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="28"/>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="28"/>
-      <c r="B9" s="28"/>
-      <c r="C9" s="34"/>
-      <c r="D9" s="29"/>
+      <c r="A9" s="27"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="28"/>
     </row>
     <row r="10" spans="1:4">
-      <c r="C10" s="34"/>
+      <c r="C10" s="33"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" firstPageNumber="2147483648" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" firstPageNumber="2147483648" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2039,40 +2064,40 @@
       <c r="B2" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="17"/>
+      <c r="H2" s="16"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" t="s">
         <v>38</v>
       </c>
-      <c r="H3" s="17"/>
+      <c r="H3" s="16"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:H3" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
@@ -2105,7 +2130,7 @@
   <sheetPr codeName="Sheet3">
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:G49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -2117,7 +2142,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="18.75"/>
   <cols>
-    <col min="1" max="1" width="16.875" style="18" customWidth="1"/>
+    <col min="1" max="1" width="16.875" style="17" customWidth="1"/>
     <col min="2" max="2" width="25.875" customWidth="1"/>
     <col min="3" max="3" width="16.875" customWidth="1"/>
     <col min="4" max="4" width="17.625" customWidth="1"/>
@@ -2150,7 +2175,7 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="17" t="s">
         <v>40</v>
       </c>
       <c r="B2" t="s">
@@ -2165,73 +2190,49 @@
       <c r="E2" t="s">
         <v>43</v>
       </c>
-      <c r="G2" s="17"/>
+      <c r="G2" s="16"/>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" t="s">
         <v>46</v>
       </c>
-      <c r="G3" s="17"/>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="C6" s="15"/>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="C7" s="15"/>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="C8" s="15"/>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="C9" s="15"/>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="C10" s="15"/>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="C11" s="15"/>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="C12" s="15"/>
+      <c r="G3" s="16"/>
     </row>
     <row r="42" spans="2:2">
-      <c r="B42" s="19"/>
+      <c r="B42" s="18"/>
     </row>
     <row r="43" spans="2:2">
-      <c r="B43" s="19"/>
+      <c r="B43" s="18"/>
     </row>
     <row r="44" spans="2:2">
-      <c r="B44" s="19"/>
+      <c r="B44" s="18"/>
     </row>
     <row r="45" spans="2:2">
-      <c r="B45" s="19"/>
+      <c r="B45" s="18"/>
     </row>
     <row r="46" spans="2:2">
-      <c r="B46" s="19"/>
+      <c r="B46" s="18"/>
     </row>
     <row r="47" spans="2:2">
-      <c r="B47" s="19"/>
+      <c r="B47" s="18"/>
     </row>
     <row r="48" spans="2:2">
-      <c r="B48" s="19"/>
-    </row>
-    <row r="49" spans="2:3">
-      <c r="B49" s="19"/>
-    </row>
-    <row r="51" spans="2:3">
-      <c r="C51" s="15"/>
+      <c r="B48" s="18"/>
+    </row>
+    <row r="49" spans="2:2">
+      <c r="B49" s="18"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:G3" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
@@ -2282,7 +2283,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="18.75"/>
   <cols>
-    <col min="1" max="1" width="16.875" style="20" customWidth="1"/>
+    <col min="1" max="1" width="16.875" style="19" customWidth="1"/>
     <col min="2" max="2" width="25.875" customWidth="1"/>
     <col min="3" max="3" width="16.875" customWidth="1"/>
     <col min="4" max="4" width="41" customWidth="1"/>
@@ -2430,15 +2431,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="D2" s="15"/>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="D3" s="15"/>
-    </row>
     <row r="4" spans="1:5">
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1">
@@ -2497,8 +2492,8 @@
     <col min="1" max="1" width="15.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="22" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:1" s="21" customFormat="1" ht="20.100000000000001" customHeight="1">
+      <c r="A1" s="21" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2829,73 +2824,73 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC785D35-B1A5-44A0-A743-865F33FA42EF}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:2" ht="18.75">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="34" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="15" t="s">
+      <c r="A2" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="15" t="s">
+      <c r="A3" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="15" t="s">
+      <c r="A4" t="s">
         <v>66</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="15" t="s">
+      <c r="A5" t="s">
         <v>68</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="15" t="s">
+      <c r="A6" t="s">
         <v>70</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="15" t="s">
+      <c r="A7" t="s">
         <v>72</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="15" t="s">
+      <c r="A8" t="s">
         <v>74</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" t="s">
         <v>73</v>
       </c>
     </row>
@@ -2904,5 +2899,6 @@
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>